<commit_message>
Fases Digestion tamaño de particula
</commit_message>
<xml_diff>
--- a/digestion.xlsx
+++ b/digestion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heber\Desktop\proyecto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D022E960-39E5-488B-BFE8-0254E0559C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7281D06C-F2DC-41F4-AD0F-E01E09514784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7E847EF5-B929-4C4B-98C1-268C9BC16A47}"/>
   </bookViews>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55198B82-300E-421F-87BA-E25D8FE3D26C}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,6 +1027,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1">
+        <f>0/60</f>
         <v>0</v>
       </c>
       <c r="E2" s="1">
@@ -1059,7 +1060,8 @@
         <v>16</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <f>10/60</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E3" s="1">
         <v>29.366666666666664</v>
@@ -1091,7 +1093,8 @@
         <v>17</v>
       </c>
       <c r="D4" s="1">
-        <v>60</v>
+        <f>60/60</f>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>25.580000000000002</v>
@@ -1123,7 +1126,8 @@
         <v>17</v>
       </c>
       <c r="D5" s="1">
-        <v>120</v>
+        <f>120/60</f>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>26.293333333333333</v>
@@ -1187,8 +1191,8 @@
         <v>20</v>
       </c>
       <c r="D7" s="1">
-        <f>D6+15</f>
-        <v>150</v>
+        <f>150/60</f>
+        <v>2.5</v>
       </c>
       <c r="E7" s="1">
         <v>26.806666666666668</v>
@@ -1220,8 +1224,8 @@
         <v>20</v>
       </c>
       <c r="D8" s="1">
-        <f>D7+15</f>
-        <v>165</v>
+        <f>165/60</f>
+        <v>2.75</v>
       </c>
       <c r="E8" s="1">
         <v>33.410000000000004</v>
@@ -1253,8 +1257,8 @@
         <v>20</v>
       </c>
       <c r="D9" s="1">
-        <f>D8+15</f>
-        <v>180</v>
+        <f>180/60</f>
+        <v>3</v>
       </c>
       <c r="E9" s="1">
         <v>26.463333333333328</v>
@@ -1286,8 +1290,8 @@
         <v>20</v>
       </c>
       <c r="D10" s="1">
-        <f>D9+15</f>
-        <v>195</v>
+        <f>195/60</f>
+        <v>3.25</v>
       </c>
       <c r="E10" s="1">
         <v>30.786666666666665</v>
@@ -1319,8 +1323,8 @@
         <v>20</v>
       </c>
       <c r="D11" s="1">
-        <f>D10+15</f>
-        <v>210</v>
+        <f>210/60</f>
+        <v>3.5</v>
       </c>
       <c r="E11" s="1">
         <v>32.273333333333333</v>
@@ -1352,8 +1356,8 @@
         <v>20</v>
       </c>
       <c r="D12" s="1">
-        <f>D11+15</f>
-        <v>225</v>
+        <f>225/60</f>
+        <v>3.75</v>
       </c>
       <c r="E12" s="1">
         <v>26.006666666666664</v>
@@ -1385,8 +1389,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="1">
-        <f>D12+15</f>
-        <v>240</v>
+        <v>4</v>
       </c>
       <c r="E13" s="1">
         <v>37.286666666666669</v>

</xml_diff>